<commit_message>
lazy guy is me
</commit_message>
<xml_diff>
--- a/variables_list_satisfaction.xlsx
+++ b/variables_list_satisfaction.xlsx
@@ -4378,9 +4378,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>cwork</t>
-  </si>
-  <si>
     <t>ann_wage</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4409,10 +4406,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Scwork</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">                     您平均每周大約花多少時間做家務工作？</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4692,6 +4685,14 @@
   </si>
   <si>
     <t>a17a | a17d | a17b | a17e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwork(delete)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scwork(delete)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4745,7 +4746,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4788,12 +4789,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -4807,7 +4802,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4831,7 +4826,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
@@ -5119,10 +5113,10 @@
   <dimension ref="A1:Y139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="V14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C89" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B32" sqref="B32"/>
+      <selection pane="bottomRight" activeCell="W24" sqref="W24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5142,8 +5136,8 @@
     <col min="17" max="18" width="9.7109375" customWidth="1"/>
     <col min="19" max="19" width="12.140625" customWidth="1"/>
     <col min="20" max="20" width="17.7109375" customWidth="1"/>
-    <col min="21" max="21" width="19.5703125" customWidth="1"/>
-    <col min="22" max="22" width="19.28515625" customWidth="1"/>
+    <col min="21" max="21" width="12.28515625" customWidth="1"/>
+    <col min="22" max="22" width="15.28515625" customWidth="1"/>
     <col min="23" max="23" width="19.7109375" customWidth="1"/>
     <col min="24" max="24" width="18.5703125" customWidth="1"/>
   </cols>
@@ -6387,7 +6381,7 @@
     </row>
     <row r="21" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>7</v>
@@ -6414,13 +6408,13 @@
         <v>1139</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="K21" t="s">
         <v>489</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>451</v>
@@ -6464,10 +6458,10 @@
     </row>
     <row r="22" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>1184</v>
+        <v>1263</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -6476,37 +6470,37 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="J22" t="s">
+        <v>1231</v>
+      </c>
+      <c r="K22" s="19" t="s">
         <v>1233</v>
-      </c>
-      <c r="K22" s="20" t="s">
-        <v>1235</v>
       </c>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="O22" s="2"/>
       <c r="P22" s="2" t="s">
+        <v>1240</v>
+      </c>
+      <c r="Q22" s="2" t="s">
         <v>1242</v>
       </c>
-      <c r="Q22" s="2" t="s">
-        <v>1244</v>
-      </c>
       <c r="R22" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="S22" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="T22" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="U22" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="V22" s="2"/>
       <c r="X22" s="8"/>
@@ -6533,11 +6527,11 @@
       <c r="G23" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="H23" s="21" t="s">
+      <c r="H23" s="20" t="s">
         <v>460</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>490</v>
@@ -6546,7 +6540,7 @@
         <v>490</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="M23" s="3" t="s">
         <v>490</v>
@@ -6607,11 +6601,11 @@
       <c r="G24" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="H24" s="21" t="s">
+      <c r="H24" s="20" t="s">
         <v>461</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>491</v>
@@ -6620,7 +6614,7 @@
         <v>491</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="M24" s="3" t="s">
         <v>491</v>
@@ -6685,7 +6679,7 @@
         <v>462</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>492</v>
@@ -6694,7 +6688,7 @@
         <v>492</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="M25" s="3" t="s">
         <v>492</v>
@@ -6762,7 +6756,7 @@
         <v>453</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="J26">
         <v>-999</v>
@@ -6771,7 +6765,7 @@
         <v>508</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="M26" s="3" t="s">
         <v>508</v>
@@ -6839,7 +6833,7 @@
         <v>463</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="J27">
         <v>-999</v>
@@ -6848,7 +6842,7 @@
         <v>509</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="M27" s="3" t="s">
         <v>509</v>
@@ -6925,7 +6919,7 @@
         <v>458</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="M28" s="3" t="s">
         <v>458</v>
@@ -7002,7 +6996,7 @@
         <v>510</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="M29" s="3" t="s">
         <v>510</v>
@@ -7046,10 +7040,10 @@
     </row>
     <row r="30" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -7061,46 +7055,46 @@
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="N30" s="2" t="s">
+        <v>1218</v>
+      </c>
+      <c r="O30" s="2" t="s">
+        <v>1218</v>
+      </c>
+      <c r="P30" s="3" t="s">
         <v>1220</v>
       </c>
-      <c r="O30" s="2" t="s">
+      <c r="Q30" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="R30" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="S30" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="T30" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="U30" s="3" t="s">
         <v>1220</v>
       </c>
-      <c r="P30" s="3" t="s">
-        <v>1222</v>
-      </c>
-      <c r="Q30" s="3" t="s">
-        <v>1220</v>
-      </c>
-      <c r="R30" s="3" t="s">
-        <v>1220</v>
-      </c>
-      <c r="S30" s="3" t="s">
-        <v>1220</v>
-      </c>
-      <c r="T30" s="3" t="s">
-        <v>1220</v>
-      </c>
-      <c r="U30" s="3" t="s">
-        <v>1222</v>
-      </c>
       <c r="V30" s="3" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="W30" s="3" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="X30" s="3" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="Y30" s="3" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="31" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
@@ -7163,8 +7157,8 @@
       <c r="A32" s="7" t="s">
         <v>921</v>
       </c>
-      <c r="B32" s="19" t="s">
-        <v>1191</v>
+      <c r="B32" s="16" t="s">
+        <v>1190</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>236</v>
@@ -7692,79 +7686,79 @@
     </row>
     <row r="43" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>1211</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>1211</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>1211</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>1212</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>1212</v>
+      </c>
+      <c r="J43" t="s">
         <v>1193</v>
       </c>
-      <c r="B43" s="16" t="s">
-        <v>1194</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>1213</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>1213</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>1213</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>1213</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>1213</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>1214</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>1214</v>
-      </c>
-      <c r="J43" t="s">
-        <v>1195</v>
-      </c>
       <c r="K43" s="2" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="L43">
         <v>-999</v>
       </c>
       <c r="M43" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="N43" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="O43" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="P43" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="Q43" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="R43" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="S43" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="T43" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="U43" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="V43" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="W43" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="X43" s="3" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="Y43" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="44" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
@@ -7802,7 +7796,7 @@
         <v>511</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="M44" s="2" t="s">
         <v>526</v>
@@ -7835,10 +7829,10 @@
         <v>699</v>
       </c>
       <c r="W44" s="2" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="X44" s="2" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="Y44" s="2" t="s">
         <v>1033</v>
@@ -7879,13 +7873,13 @@
         <v>663</v>
       </c>
       <c r="T45" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="U45" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="V45" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="W45" s="1" t="s">
         <v>768</v>
@@ -8127,7 +8121,7 @@
     </row>
     <row r="49" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>68</v>
@@ -8154,13 +8148,13 @@
         <v>498</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="K49" t="s">
         <v>514</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="M49" s="2" t="s">
         <v>528</v>
@@ -8204,10 +8198,10 @@
     </row>
     <row r="50" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>1192</v>
+        <v>1264</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -8216,37 +8210,37 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
       <c r="I50" s="2" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="J50" s="2" t="s">
+        <v>1232</v>
+      </c>
+      <c r="K50" t="s">
         <v>1234</v>
-      </c>
-      <c r="K50" t="s">
-        <v>1236</v>
       </c>
       <c r="L50" s="3"/>
       <c r="M50" s="2"/>
       <c r="N50" s="8" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="O50" s="8"/>
       <c r="P50" s="17" t="s">
+        <v>1241</v>
+      </c>
+      <c r="Q50" s="8" t="s">
         <v>1243</v>
       </c>
-      <c r="Q50" s="8" t="s">
-        <v>1245</v>
-      </c>
       <c r="R50" s="2" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="S50" s="2" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="T50" s="2" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="U50" s="2" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="W50" s="2"/>
       <c r="Y50" s="2"/>
@@ -8273,7 +8267,7 @@
       <c r="G51" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="H51" s="21" t="s">
+      <c r="H51" s="20" t="s">
         <v>38</v>
       </c>
       <c r="I51" s="2" t="s">
@@ -8286,7 +8280,7 @@
         <v>515</v>
       </c>
       <c r="L51" s="3" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="M51" s="2" t="s">
         <v>529</v>
@@ -8347,7 +8341,7 @@
       <c r="G52" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="H52" s="21" t="s">
+      <c r="H52" s="20" t="s">
         <v>39</v>
       </c>
       <c r="I52" s="3" t="s">
@@ -8360,7 +8354,7 @@
         <v>516</v>
       </c>
       <c r="L52" s="3" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="M52" s="3" t="s">
         <v>530</v>
@@ -8784,10 +8778,10 @@
     </row>
     <row r="58" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -8799,43 +8793,43 @@
       <c r="K58" s="2"/>
       <c r="L58" s="3"/>
       <c r="M58" s="3" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="N58" s="2" t="s">
+        <v>1219</v>
+      </c>
+      <c r="O58" s="2" t="s">
+        <v>1219</v>
+      </c>
+      <c r="P58" s="2" t="s">
+        <v>1215</v>
+      </c>
+      <c r="Q58" s="2" t="s">
+        <v>1219</v>
+      </c>
+      <c r="R58" s="2" t="s">
+        <v>1219</v>
+      </c>
+      <c r="S58" s="2" t="s">
+        <v>1219</v>
+      </c>
+      <c r="T58" s="2" t="s">
+        <v>1219</v>
+      </c>
+      <c r="U58" s="2" t="s">
+        <v>1215</v>
+      </c>
+      <c r="V58" s="2" t="s">
+        <v>1219</v>
+      </c>
+      <c r="W58" s="2" t="s">
         <v>1221</v>
       </c>
-      <c r="O58" s="2" t="s">
+      <c r="X58" s="2" t="s">
         <v>1221</v>
       </c>
-      <c r="P58" s="2" t="s">
-        <v>1217</v>
-      </c>
-      <c r="Q58" s="2" t="s">
+      <c r="Y58" s="2" t="s">
         <v>1221</v>
-      </c>
-      <c r="R58" s="2" t="s">
-        <v>1221</v>
-      </c>
-      <c r="S58" s="2" t="s">
-        <v>1221</v>
-      </c>
-      <c r="T58" s="2" t="s">
-        <v>1221</v>
-      </c>
-      <c r="U58" s="2" t="s">
-        <v>1217</v>
-      </c>
-      <c r="V58" s="2" t="s">
-        <v>1221</v>
-      </c>
-      <c r="W58" s="2" t="s">
-        <v>1223</v>
-      </c>
-      <c r="X58" s="2" t="s">
-        <v>1223</v>
-      </c>
-      <c r="Y58" s="2" t="s">
-        <v>1223</v>
       </c>
     </row>
     <row r="59" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
@@ -8969,79 +8963,79 @@
     </row>
     <row r="65" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="I65" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="L65">
         <v>-999</v>
       </c>
       <c r="M65" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="N65" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="O65" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="P65" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="Q65" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="R65" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="S65" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="T65" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="U65" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="V65" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="W65" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="X65" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="Y65" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="66" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
@@ -10128,7 +10122,7 @@
         <v>626</v>
       </c>
       <c r="Q100" s="2" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="V100" t="s">
         <v>722</v>
@@ -10481,10 +10475,10 @@
     </row>
     <row r="108" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A108" s="14" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
@@ -10773,10 +10767,10 @@
     </row>
     <row r="114" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A114" s="14" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
@@ -11065,10 +11059,10 @@
     </row>
     <row r="120" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A120" s="14" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="C120" s="2"/>
       <c r="D120" s="2"/>
@@ -11357,10 +11351,10 @@
     </row>
     <row r="126" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A126" s="14" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="C126" s="2"/>
       <c r="D126" s="2"/>
@@ -11590,10 +11584,10 @@
     </row>
     <row r="132" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A132" s="14" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="C132" s="2"/>
       <c r="D132" s="2"/>
@@ -11811,10 +11805,10 @@
     </row>
     <row r="138" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A138" s="14" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="C138" s="2"/>
       <c r="D138" s="2"/>

</xml_diff>